<commit_message>
Cambio de nombre de productos
</commit_message>
<xml_diff>
--- a/Inserts.xlsx
+++ b/Inserts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="745" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="745" firstSheet="10" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="sd_usuario" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="389">
   <si>
     <t>nombres</t>
   </si>
@@ -1191,6 +1191,18 @@
   </si>
   <si>
     <t>recogida</t>
+  </si>
+  <si>
+    <t>LORETO</t>
+  </si>
+  <si>
+    <t>JULIACA</t>
+  </si>
+  <si>
+    <t>OROYA</t>
+  </si>
+  <si>
+    <t>peso_unidad</t>
   </si>
 </sst>
 </file>
@@ -2442,7 +2454,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2781,7 +2793,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:H26"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4796,7 +4808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5:I9"/>
     </sheetView>
   </sheetViews>
@@ -5178,8 +5190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5226,7 +5238,7 @@
         <v>8421</v>
       </c>
       <c r="F2" t="str">
-        <f>"INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES ("&amp;B2&amp;",'"&amp;C2&amp;"','"&amp;E2&amp;"',1,sysdate(),'admin');"</f>
+        <f t="shared" ref="F2:F13" si="0">"INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES ("&amp;B2&amp;",'"&amp;C2&amp;"','"&amp;E2&amp;"',1,sysdate(),'admin');"</f>
         <v>INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES (1,'2024-10-04','8421',1,sysdate(),'admin');</v>
       </c>
     </row>
@@ -5248,7 +5260,7 @@
         <v>1269</v>
       </c>
       <c r="F3" t="str">
-        <f>"INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES ("&amp;B3&amp;",'"&amp;C3&amp;"','"&amp;E3&amp;"',1,sysdate(),'admin');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES (2,'2025-03-06','1269',1,sysdate(),'admin');</v>
       </c>
     </row>
@@ -5270,7 +5282,7 @@
         <v>4589</v>
       </c>
       <c r="F4" t="str">
-        <f>"INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES ("&amp;B4&amp;",'"&amp;C4&amp;"','"&amp;E4&amp;"',1,sysdate(),'admin');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES (3,'2024-08-14','4589',1,sysdate(),'admin');</v>
       </c>
     </row>
@@ -5292,7 +5304,7 @@
         <v>3586</v>
       </c>
       <c r="F5" t="str">
-        <f>"INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES ("&amp;B5&amp;",'"&amp;C5&amp;"','"&amp;E5&amp;"',1,sysdate(),'admin');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES (4,'2024-01-28','3586',1,sysdate(),'admin');</v>
       </c>
     </row>
@@ -5314,7 +5326,7 @@
         <v>3458</v>
       </c>
       <c r="F6" t="str">
-        <f>"INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES ("&amp;B6&amp;",'"&amp;C6&amp;"','"&amp;E6&amp;"',1,sysdate(),'admin');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES (9,'2025-01-14','3458',1,sysdate(),'admin');</v>
       </c>
     </row>
@@ -5336,7 +5348,7 @@
         <v>8547</v>
       </c>
       <c r="F7" t="str">
-        <f>"INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES ("&amp;B7&amp;",'"&amp;C7&amp;"','"&amp;E7&amp;"',1,sysdate(),'admin');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES (10,'2025-08-14','8547',1,sysdate(),'admin');</v>
       </c>
     </row>
@@ -5358,7 +5370,7 @@
         <v>3138</v>
       </c>
       <c r="F8" t="str">
-        <f>"INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES ("&amp;B8&amp;",'"&amp;C8&amp;"','"&amp;E8&amp;"',1,sysdate(),'admin');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES (11,'2024-11-23','3138',1,sysdate(),'admin');</v>
       </c>
     </row>
@@ -5380,29 +5392,29 @@
         <v>9521</v>
       </c>
       <c r="F9" t="str">
-        <f>"INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES ("&amp;B9&amp;",'"&amp;C9&amp;"','"&amp;E9&amp;"',1,sysdate(),'admin');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES (12,'2025-01-14','9521',1,sysdate(),'admin');</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="15">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="15">
         <v>17</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="D10" s="20" t="str">
+      <c r="D10" s="22" t="str">
         <f>VLOOKUP(B10,sd_usuario!$B$2:$F$25,5,0)</f>
         <v>01248755</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="22">
         <v>2415</v>
       </c>
-      <c r="F10" t="str">
-        <f>"INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES ("&amp;B10&amp;",'"&amp;C10&amp;"','"&amp;E10&amp;"',1,sysdate(),'admin');"</f>
+      <c r="F10" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES (17,'2025-02-25','2415',1,sysdate(),'admin');</v>
       </c>
     </row>
@@ -5424,51 +5436,51 @@
         <v>2205</v>
       </c>
       <c r="F11" s="15" t="str">
-        <f>"INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES ("&amp;B11&amp;",'"&amp;C11&amp;"','"&amp;E11&amp;"',1,sysdate(),'admin');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES (18,'2025-04-14','2205',1,sysdate(),'admin');</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="15">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="15">
         <v>19</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="D12" s="20" t="str">
+      <c r="D12" s="22" t="str">
         <f>VLOOKUP(B12,sd_usuario!$B$2:$F$25,5,0)</f>
         <v>12457845</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="22">
         <v>6982</v>
       </c>
-      <c r="F12" t="str">
-        <f>"INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES ("&amp;B12&amp;",'"&amp;C12&amp;"','"&amp;E12&amp;"',1,sysdate(),'admin');"</f>
+      <c r="F12" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES (19,'2024-10-21','6982',1,sysdate(),'admin');</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="15">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="15">
         <v>20</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="D13" s="20" t="str">
+      <c r="D13" s="22" t="str">
         <f>VLOOKUP(B13,sd_usuario!$B$2:$F$25,5,0)</f>
         <v>15655845</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="22">
         <v>2492</v>
       </c>
-      <c r="F13" t="str">
-        <f>"INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES ("&amp;B13&amp;",'"&amp;C13&amp;"','"&amp;E13&amp;"',1,sysdate(),'admin');"</f>
+      <c r="F13" s="15" t="str">
+        <f t="shared" si="0"/>
         <v>INSERT INTO sd_conductor(id_usuario, fecha_venc_licencia, clave_digital, activo, fecha_registro, usuario_registro) VALUES (20,'2024-07-06','2492',1,sysdate(),'admin');</v>
       </c>
     </row>
@@ -5691,7 +5703,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C2:C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5753,7 +5765,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5774,11 +5786,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>385</v>
       </c>
       <c r="C2" t="str">
         <f>"INSERT INTO sd_marca("&amp;$B$1&amp;", activo, fecha_registro, usuario_registro) VALUES ('"&amp;B2&amp;"',1,sysdate(),'admin');"</f>
-        <v>INSERT INTO sd_marca(nombre, activo, fecha_registro, usuario_registro) VALUES ('APU',1,sysdate(),'admin');</v>
+        <v>INSERT INTO sd_marca(nombre, activo, fecha_registro, usuario_registro) VALUES ('LORETO',1,sysdate(),'admin');</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -5786,11 +5798,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>387</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C7" si="0">"INSERT INTO sd_marca("&amp;$B$1&amp;", activo, fecha_registro, usuario_registro) VALUES ('"&amp;B3&amp;"',1,sysdate(),'admin');"</f>
-        <v>INSERT INTO sd_marca(nombre, activo, fecha_registro, usuario_registro) VALUES ('SOL',1,sysdate(),'admin');</v>
+        <v>INSERT INTO sd_marca(nombre, activo, fecha_registro, usuario_registro) VALUES ('OROYA',1,sysdate(),'admin');</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -5798,11 +5810,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>386</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO sd_marca(nombre, activo, fecha_registro, usuario_registro) VALUES ('PIRAMIDE',1,sysdate(),'admin');</v>
+        <v>INSERT INTO sd_marca(nombre, activo, fecha_registro, usuario_registro) VALUES ('JULIACA',1,sysdate(),'admin');</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -5925,20 +5937,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="14.77734375" style="2" customWidth="1"/>
+    <col min="3" max="6" width="14.77734375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>74</v>
       </c>
@@ -5952,13 +5964,16 @@
         <v>69</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5972,14 +5987,17 @@
         <v>1</v>
       </c>
       <c r="E2" s="9">
+        <v>42.5</v>
+      </c>
+      <c r="F2" s="9">
         <v>10000</v>
       </c>
-      <c r="F2" t="str">
-        <f>"INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES ("&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;",1,sysdate(),'admin');"</f>
-        <v>INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES (1,1,1,10000,1,sysdate(),'admin');</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G2" t="str">
+        <f>"INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, peso_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES ("&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;", "&amp;F2&amp;",1,sysdate(),'admin');"</f>
+        <v>INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, peso_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES (1,1,1,42.5, 10000,1,sysdate(),'admin');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5993,14 +6011,17 @@
         <v>2</v>
       </c>
       <c r="E3" s="9">
+        <v>52.5</v>
+      </c>
+      <c r="F3" s="9">
         <v>15000</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F7" si="0">"INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES ("&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;",1,sysdate(),'admin');"</f>
-        <v>INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES (1,2,2,15000,1,sysdate(),'admin');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G7" si="0">"INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, peso_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES ("&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;", "&amp;F3&amp;",1,sysdate(),'admin');"</f>
+        <v>INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, peso_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES (1,2,2,52.5, 15000,1,sysdate(),'admin');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -6014,14 +6035,17 @@
         <v>3</v>
       </c>
       <c r="E4" s="9">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9">
         <v>12000</v>
       </c>
-      <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES (2,3,3,12000,1,sysdate(),'admin');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, peso_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES (2,3,3,5, 12000,1,sysdate(),'admin');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -6035,14 +6059,17 @@
         <v>3</v>
       </c>
       <c r="E5" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="F5" s="9">
         <v>18000</v>
       </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES (2,5,3,18000,1,sysdate(),'admin');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, peso_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES (2,5,3,3.5, 18000,1,sysdate(),'admin');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>79</v>
       </c>
@@ -6056,14 +6083,17 @@
         <v>4</v>
       </c>
       <c r="E6" s="9">
+        <v>8</v>
+      </c>
+      <c r="F6" s="9">
         <v>8000</v>
       </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES (3,4,4,8000,1,sysdate(),'admin');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, peso_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES (3,4,4,8, 8000,1,sysdate(),'admin');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>81</v>
       </c>
@@ -6077,111 +6107,108 @@
         <v>4</v>
       </c>
       <c r="E7" s="9">
+        <v>9</v>
+      </c>
+      <c r="F7" s="9">
         <v>13500</v>
       </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES (3,6,4,13500,1,sysdate(),'admin');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" t="str">
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO sd_producto_venta (id_producto, id_marca, id_unidad, peso_unidad, stock_actual, activo, fecha_registro, usuario_registro) VALUES (3,6,4,9, 13500,1,sysdate(),'admin');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" t="str">
         <f>VLOOKUP(B2,sd_producto!$A$2:$B$4,2,0)</f>
         <v>Cemento</v>
       </c>
-      <c r="H8" t="str">
-        <f>VLOOKUP(C2,sd_marca!$A$2:$B$7,2,0)</f>
-        <v>APU</v>
-      </c>
-      <c r="I8" t="str">
+      <c r="I8" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="J8" t="str">
         <f>VLOOKUP(D2,sd_unidad!$A$2:$B$7,2,0)</f>
         <v>bolsas de 42.5 kg</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F9" s="2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G9" s="2">
         <v>2</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <f>VLOOKUP(B3,sd_producto!$A$2:$B$4,2,0)</f>
         <v>Cemento</v>
       </c>
-      <c r="H9" t="str">
-        <f>VLOOKUP(C3,sd_marca!$A$2:$B$7,2,0)</f>
-        <v>SOL</v>
-      </c>
-      <c r="I9" t="str">
+      <c r="I9" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="J9" t="str">
         <f>VLOOKUP(D3,sd_unidad!$A$2:$B$7,2,0)</f>
         <v>bolsas de 52.5 kg</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F10" s="2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G10" s="2">
         <v>3</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <f>VLOOKUP(B4,sd_producto!$A$2:$B$4,2,0)</f>
         <v>Ladrillo</v>
       </c>
-      <c r="H10" t="str">
-        <f>VLOOKUP(C4,sd_marca!$A$2:$B$7,2,0)</f>
-        <v>PIRAMIDE</v>
-      </c>
-      <c r="I10" t="str">
+      <c r="I10" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="J10" t="str">
         <f>VLOOKUP(D4,sd_unidad!$A$2:$B$7,2,0)</f>
         <v>ladrillos</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F11" s="2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G11" s="2">
         <v>4</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <f>VLOOKUP(B5,sd_producto!$A$2:$B$4,2,0)</f>
         <v>Ladrillo</v>
       </c>
-      <c r="H11" t="str">
-        <f>VLOOKUP(C5,sd_marca!$A$2:$B$7,2,0)</f>
-        <v>LARK</v>
-      </c>
-      <c r="I11" t="str">
+      <c r="I11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" t="str">
         <f>VLOOKUP(D5,sd_unidad!$A$2:$B$7,2,0)</f>
         <v>ladrillos</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F12" s="2" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" t="str">
         <f>VLOOKUP(B6,sd_producto!$A$2:$B$4,2,0)</f>
         <v>Pallets</v>
       </c>
-      <c r="H12" t="str">
-        <f>VLOOKUP(C6,sd_marca!$A$2:$B$7,2,0)</f>
-        <v>BASA</v>
-      </c>
-      <c r="I12" t="str">
+      <c r="I12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" t="str">
         <f>VLOOKUP(D6,sd_unidad!$A$2:$B$7,2,0)</f>
         <v>pallets</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F13" s="2" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" t="str">
         <f>VLOOKUP(B7,sd_producto!$A$2:$B$4,2,0)</f>
         <v>Pallets</v>
       </c>
-      <c r="H13" t="str">
-        <f>VLOOKUP(C7,sd_marca!$A$2:$B$7,2,0)</f>
-        <v>CHEP</v>
-      </c>
-      <c r="I13" t="str">
+      <c r="I13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" t="str">
         <f>VLOOKUP(D7,sd_unidad!$A$2:$B$7,2,0)</f>
         <v>pallets</v>
       </c>

</xml_diff>

<commit_message>
Inicio del revisor completo
</commit_message>
<xml_diff>
--- a/Inserts.xlsx
+++ b/Inserts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="745" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="745" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sd_usuario" sheetId="1" r:id="rId1"/>
@@ -5296,7 +5296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -5599,7 +5599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Carga de productos terminada
</commit_message>
<xml_diff>
--- a/Inserts.xlsx
+++ b/Inserts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="745" firstSheet="15" activeTab="22"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="745" firstSheet="14" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="sd_usuario" sheetId="1" r:id="rId1"/>
@@ -4043,8 +4043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5730,7 +5730,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6053,8 +6053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6150,6 +6150,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Pesaje lleno y salida
</commit_message>
<xml_diff>
--- a/Inserts.xlsx
+++ b/Inserts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="745" firstSheet="14" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="745" firstSheet="7" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="sd_usuario" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="443">
   <si>
     <t>nombres</t>
   </si>
@@ -1300,9 +1300,6 @@
     <t>Despacho</t>
   </si>
   <si>
-    <t>Peso</t>
-  </si>
-  <si>
     <t>15500</t>
   </si>
   <si>
@@ -1334,13 +1331,56 @@
   </si>
   <si>
     <t>NFESIFNML</t>
+  </si>
+  <si>
+    <t>valor_pesaje_vacio</t>
+  </si>
+  <si>
+    <t>valor_pesaje_lleno</t>
+  </si>
+  <si>
+    <t>Peso vehiculo</t>
+  </si>
+  <si>
+    <t>Peso carga</t>
+  </si>
+  <si>
+    <t>desfase</t>
+  </si>
+  <si>
+    <t>qr_entrada</t>
+  </si>
+  <si>
+    <t>qr_salida</t>
+  </si>
+  <si>
+    <t>JKSAFNAJFK</t>
+  </si>
+  <si>
+    <t>FIOESNFKL</t>
+  </si>
+  <si>
+    <t>MIFOEMFS</t>
+  </si>
+  <si>
+    <t>IMDOSMVSD</t>
+  </si>
+  <si>
+    <t>MFIFODSMV</t>
+  </si>
+  <si>
+    <t>FSMVIODSVQ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1370,8 +1410,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1396,6 +1443,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1406,11 +1459,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1458,9 +1512,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2941,8 +3002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:G5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3747,6 +3808,12 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>1350</v>
+      </c>
+      <c r="F29">
+        <v>6</v>
+      </c>
       <c r="G29">
         <v>2</v>
       </c>
@@ -3823,10 +3890,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3837,7 +3904,7 @@
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>160</v>
       </c>
@@ -3878,10 +3945,16 @@
         <v>169</v>
       </c>
       <c r="N1" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3918,15 +3991,21 @@
       <c r="L2" s="8">
         <v>0</v>
       </c>
-      <c r="M2" s="8">
-        <v>20</v>
-      </c>
-      <c r="N2" t="str">
-        <f>"INSERT INTO sd_planta ("&amp;$B$1&amp;", "&amp;$C$1&amp;","&amp;$D$1&amp;","&amp;$E$1&amp;", "&amp;$F$1&amp;","&amp;$G$1&amp;", "&amp;$H$1&amp;","&amp;$I$1&amp;", "&amp;$J$1&amp;","&amp;$K$1&amp;", "&amp;$L$1&amp;", "&amp;$M$1&amp;",activo, fecha_registro, usuario_registro) VALUES ('"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"',"&amp;E2&amp;", "&amp;F2&amp;", "&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;", "&amp;L2&amp;", "&amp;M2&amp;", 1,sysdate(),'admin');"</f>
-        <v>INSERT INTO sd_planta (nombre, direccion,distrito,capacidad_maxima, ubicacion_x1,ubicacion_x2, ubicacion_y1,ubicacion_y2, limite_inf_pesaje_antes,limite_sup_pesaje_antes, limite_inf_pesaje_despues, limite_sup_pesaje_despues,activo, fecha_registro, usuario_registro) VALUES ('Planta Lima Sur','Av. Las Malvinas 4589','San Juan de Miraflores',60, 10.1, 11.1, 24.5, 26.5, 300, 300, 0, 20, 1,sysdate(),'admin');</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M2" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="N2" s="35" t="s">
+        <v>437</v>
+      </c>
+      <c r="O2" s="35" t="s">
+        <v>440</v>
+      </c>
+      <c r="P2" t="str">
+        <f>"INSERT INTO sd_planta ("&amp;$B$1&amp;", "&amp;$C$1&amp;","&amp;$D$1&amp;","&amp;$E$1&amp;", "&amp;$F$1&amp;","&amp;$G$1&amp;", "&amp;$H$1&amp;","&amp;$I$1&amp;", "&amp;$J$1&amp;","&amp;$K$1&amp;", "&amp;$L$1&amp;", "&amp;$M$1&amp;", "&amp;N1&amp;", "&amp;O1&amp;", activo, fecha_registro, usuario_registro) VALUES ('"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"',"&amp;E2&amp;", "&amp;F2&amp;", "&amp;G2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;", "&amp;L2&amp;", "&amp;M2&amp;", '"&amp;N2&amp;"', '"&amp;O2&amp;"', 1,sysdate(),'admin');"</f>
+        <v>INSERT INTO sd_planta (nombre, direccion,distrito,capacidad_maxima, ubicacion_x1,ubicacion_x2, ubicacion_y1,ubicacion_y2, limite_inf_pesaje_antes,limite_sup_pesaje_antes, limite_inf_pesaje_despues, limite_sup_pesaje_despues, qr_entrada, qr_salida, activo, fecha_registro, usuario_registro) VALUES ('Planta Lima Sur','Av. Las Malvinas 4589','San Juan de Miraflores',60, 10.1, 11.1, 24.5, 26.5, 300, 300, 0, 0.5, 'JKSAFNAJFK', 'IMDOSMVSD', 1,sysdate(),'admin');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3965,15 +4044,21 @@
       <c r="L3" s="8">
         <v>0</v>
       </c>
-      <c r="M3" s="8">
-        <v>20</v>
-      </c>
-      <c r="N3" t="str">
-        <f t="shared" ref="N3:N4" si="0">"INSERT INTO sd_planta ("&amp;$B$1&amp;", "&amp;$C$1&amp;","&amp;$D$1&amp;","&amp;$E$1&amp;", "&amp;$F$1&amp;","&amp;$G$1&amp;", "&amp;$H$1&amp;","&amp;$I$1&amp;", "&amp;$J$1&amp;","&amp;$K$1&amp;", "&amp;$L$1&amp;", "&amp;$M$1&amp;",activo, fecha_registro, usuario_registro) VALUES ('"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"',"&amp;E3&amp;", "&amp;F3&amp;", "&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;", "&amp;L3&amp;", "&amp;M3&amp;", 1,sysdate(),'admin');"</f>
-        <v>INSERT INTO sd_planta (nombre, direccion,distrito,capacidad_maxima, ubicacion_x1,ubicacion_x2, ubicacion_y1,ubicacion_y2, limite_inf_pesaje_antes,limite_sup_pesaje_antes, limite_inf_pesaje_despues, limite_sup_pesaje_despues,activo, fecha_registro, usuario_registro) VALUES ('Planta Lima Norte','Av. Tulipanes 1248','Ancón',50, 12.5, 13.5, 27.5, 29.5, 320, 300, 0, 20, 1,sysdate(),'admin');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M3" s="35">
+        <v>0.4</v>
+      </c>
+      <c r="N3" s="35" t="s">
+        <v>438</v>
+      </c>
+      <c r="O3" s="35" t="s">
+        <v>441</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:P4" si="0">"INSERT INTO sd_planta ("&amp;$B$1&amp;", "&amp;$C$1&amp;","&amp;$D$1&amp;","&amp;$E$1&amp;", "&amp;$F$1&amp;","&amp;$G$1&amp;", "&amp;$H$1&amp;","&amp;$I$1&amp;", "&amp;$J$1&amp;","&amp;$K$1&amp;", "&amp;$L$1&amp;", "&amp;$M$1&amp;", "&amp;N2&amp;", "&amp;O2&amp;", activo, fecha_registro, usuario_registro) VALUES ('"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"',"&amp;E3&amp;", "&amp;F3&amp;", "&amp;G3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;", "&amp;L3&amp;", "&amp;M3&amp;", '"&amp;N3&amp;"', '"&amp;O3&amp;"', 1,sysdate(),'admin');"</f>
+        <v>INSERT INTO sd_planta (nombre, direccion,distrito,capacidad_maxima, ubicacion_x1,ubicacion_x2, ubicacion_y1,ubicacion_y2, limite_inf_pesaje_antes,limite_sup_pesaje_antes, limite_inf_pesaje_despues, limite_sup_pesaje_despues, JKSAFNAJFK, IMDOSMVSD, activo, fecha_registro, usuario_registro) VALUES ('Planta Lima Norte','Av. Tulipanes 1248','Ancón',50, 12.5, 13.5, 27.5, 29.5, 320, 300, 0, 0.4, 'FIOESNFKL', 'MFIFODSMV', 1,sysdate(),'admin');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4011,15 +4096,21 @@
       <c r="L4" s="8">
         <v>0</v>
       </c>
-      <c r="M4" s="8">
-        <v>18</v>
-      </c>
-      <c r="N4" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO sd_planta (nombre, direccion,distrito,capacidad_maxima, ubicacion_x1,ubicacion_x2, ubicacion_y1,ubicacion_y2, limite_inf_pesaje_antes,limite_sup_pesaje_antes, limite_inf_pesaje_despues, limite_sup_pesaje_despues,activo, fecha_registro, usuario_registro) VALUES ('Planta Lima Este','Av. Juliaca 3458','Ate',40, 7, 8, 22.5, 24, 300, 300, 0, 18, 1,sysdate(),'admin');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M4" s="35">
+        <v>0.3</v>
+      </c>
+      <c r="N4" s="35" t="s">
+        <v>439</v>
+      </c>
+      <c r="O4" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO sd_planta (nombre, direccion,distrito,capacidad_maxima, ubicacion_x1,ubicacion_x2, ubicacion_y1,ubicacion_y2, limite_inf_pesaje_antes,limite_sup_pesaje_antes, limite_inf_pesaje_despues, limite_sup_pesaje_despues, FIOESNFKL, MFIFODSMV, activo, fecha_registro, usuario_registro) VALUES ('Planta Lima Este','Av. Juliaca 3458','Ate',40, 7, 8, 22.5, 24, 300, 300, 0, 0.3, 'MIFOEMFS', 'FSMVIODSVQ', 1,sysdate(),'admin');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -4032,6 +4123,8 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4044,7 +4137,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="A8:B8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4185,7 +4278,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="36" t="s">
         <v>181</v>
       </c>
       <c r="C12" t="str">
@@ -5780,10 +5873,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F7"/>
+      <selection activeCell="B5" sqref="B5:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5937,6 +6030,7 @@
         <v>INSERT INTO sd_zona_balanza (id_tipo_pesaje, id_planta, codigo, contrasena, activo, usuario_registro, fecha_registro) VALUES (2, 1,'B6', 'balanza6', 1, 'admin', sysdate());</v>
       </c>
     </row>
+    <row r="29" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5948,7 +6042,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6054,14 +6148,14 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B1" t="s">
         <v>160</v>
@@ -6084,10 +6178,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E2" t="str">
         <f>"INSERT INTO sd_canal_carga (id_planta, codigo, qr_fisico, activo, usuario_registro, fecha_registro ) VALUES ("&amp;B2&amp;", '"&amp;C2&amp;"', '"&amp;D2&amp;"', 1, 'admin', sysdate());"</f>
@@ -6102,10 +6196,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E5" si="0">"INSERT INTO sd_canal_carga (id_planta, codigo, qr_fisico, activo, usuario_registro, fecha_registro ) VALUES ("&amp;B3&amp;", '"&amp;C3&amp;"', '"&amp;D3&amp;"', 1, 'admin', sysdate());"</f>
@@ -6120,10 +6214,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -6138,10 +6232,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -6657,7 +6751,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G2:G7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6989,7 +7083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
@@ -6999,7 +7093,9 @@
     <col min="2" max="2" width="14.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="14.77734375" style="2" customWidth="1"/>
     <col min="8" max="8" width="20.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="20.77734375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="20.77734375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -7757,51 +7853,128 @@
         <v>INSERT INTO sd_vehiculo(id_tipo_vehiculo, placa, largo, ancho, altura, peso, fecha_venc_circulacion, tiene_tarjeta_propiedad, fecha_venc_soat, activo, fecha_registro, usuario_registro) values (2,'O3B-647',48,2.4,2,5500,'2025-08-17',1,'2025-03-09',1,sysdate(),'admin');</v>
       </c>
     </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33" t="s">
+        <v>414</v>
+      </c>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+    </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E25" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="I25" s="2" t="s">
+      <c r="B25" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>417</v>
+      </c>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33" t="s">
+        <v>420</v>
+      </c>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="33" t="s">
+        <v>415</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="33" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E26" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>414</v>
+      <c r="G26" s="34">
+        <f>1350*9</f>
+        <v>12150</v>
+      </c>
+      <c r="H26" s="33">
+        <v>15480.45</v>
+      </c>
+      <c r="I26" s="13">
+        <f>H26+G26+10</f>
+        <v>27640.45</v>
+      </c>
+      <c r="J26" s="13">
+        <f>I26-H26-G26</f>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E27" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>421</v>
-      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E28" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>420</v>
-      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13">
+        <f>(I26-H26)/1350</f>
+        <v>9.007407407407408</v>
+      </c>
+      <c r="J28" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>